<commit_message>
Add verifying up serial number
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prmagnata\Documents\Git\erdd-erdi.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BF320D-E45B-43A7-8BC5-EB7DB204F5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76490EF0-BCB5-407F-A7A7-C5A79648790B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="17190" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>